<commit_message>
calculated rydberg constant to 0.03 percent error!!!!!!
</commit_message>
<xml_diff>
--- a/Hydrogen.xlsx
+++ b/Hydrogen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Intermediate Lab\Intermediate-Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2ABFEBAE-42D8-4A45-88D2-6DBCE174BAFE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{81FC21C0-0151-4E2F-A204-3FE7C905E031}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>order</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>zero</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -887,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -903,7 +906,7 @@
     <col min="8" max="8" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,8 +934,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -960,8 +966,11 @@
       <c r="I2">
         <v>1.5</v>
       </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -989,8 +998,11 @@
       <c r="I3">
         <v>1.5</v>
       </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1018,8 +1030,11 @@
       <c r="I4">
         <v>1.5</v>
       </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1047,8 +1062,11 @@
       <c r="I5">
         <v>1.5</v>
       </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1076,8 +1094,11 @@
       <c r="I6">
         <v>1.5</v>
       </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1105,8 +1126,11 @@
       <c r="I7">
         <v>1.5</v>
       </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1134,8 +1158,11 @@
       <c r="I8">
         <v>1.5</v>
       </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1163,8 +1190,11 @@
       <c r="I9">
         <v>1.5</v>
       </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1192,8 +1222,11 @@
       <c r="I10">
         <v>1.5</v>
       </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1221,8 +1254,11 @@
       <c r="I11">
         <v>1.5</v>
       </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1250,8 +1286,11 @@
       <c r="I12">
         <v>1.5</v>
       </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1278,6 +1317,9 @@
       </c>
       <c r="I13">
         <v>1.5</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>